<commit_message>
docker, protocol bug bixes
</commit_message>
<xml_diff>
--- a/protocol/MF6pt2.xlsx
+++ b/protocol/MF6pt2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo-Tyres\protocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9ED3ED-7559-462E-B3F7-42545CC93B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBFE56B-0B94-4723-AC99-BB71EB076AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MF6.2" sheetId="12" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="30">
   <si>
     <t>Combined</t>
   </si>
@@ -115,15 +115,6 @@
   </si>
   <si>
     <t>-SR</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>L6</t>
   </si>
 </sst>
 </file>
@@ -561,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58031019-AFD2-4461-8B24-C325E2174DEC}">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H195" sqref="H195"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1591,7 +1582,7 @@
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -1617,7 +1608,7 @@
         <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>25</v>
@@ -1643,7 +1634,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>25</v>
@@ -1669,7 +1660,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>24</v>
@@ -1695,7 +1686,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
test: dependency execution, backtracking, abaqus
</commit_message>
<xml_diff>
--- a/protocol/MF6pt2.xlsx
+++ b/protocol/MF6pt2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo-Tyres\protocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687C9AA7-0E23-4151-A7B0-0FD627960685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A2A243-3682-4906-9BA9-451B1A53AEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="56">
   <si>
     <t>Combined</t>
   </si>
@@ -127,6 +127,72 @@
   </si>
   <si>
     <t>Old Job</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac1</t>
+  </si>
+  <si>
+    <t>rollingtire_freeroll</t>
+  </si>
+  <si>
+    <t>tiretransfer_axi_half</t>
+  </si>
+  <si>
+    <t>tiretransfer_full</t>
+  </si>
+  <si>
+    <t>tiretransfer_node</t>
+  </si>
+  <si>
+    <t>tiretransfer_symmetric</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac2</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac3</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac4</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac5</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac6</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac7</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac8</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac9</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac10</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac11</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac12</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac13</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac14</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac15</t>
+  </si>
+  <si>
+    <t>rollingtire_brake_trac16</t>
   </si>
 </sst>
 </file>
@@ -564,9 +630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58031019-AFD2-4461-8B24-C325E2174DEC}">
   <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,6 +646,7 @@
     <col min="7" max="7" width="16.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.44140625" customWidth="1"/>
+    <col min="10" max="10" width="24.77734375" customWidth="1"/>
     <col min="14" max="14" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -655,10 +722,10 @@
         <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -687,10 +754,10 @@
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -719,10 +786,10 @@
         <v>22</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -751,10 +818,10 @@
         <v>22</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -783,10 +850,10 @@
         <v>22</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -815,10 +882,10 @@
         <v>22</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -847,10 +914,10 @@
         <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -879,10 +946,10 @@
         <v>22</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -911,10 +978,10 @@
         <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -943,10 +1010,10 @@
         <v>22</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -975,10 +1042,10 @@
         <v>22</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1007,10 +1074,10 @@
         <v>22</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1039,10 +1106,10 @@
         <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1071,10 +1138,10 @@
         <v>22</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1103,10 +1170,10 @@
         <v>22</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1135,10 +1202,10 @@
         <v>22</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1167,10 +1234,10 @@
         <v>22</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1199,10 +1266,10 @@
         <v>22</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1231,10 +1298,10 @@
         <v>22</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1263,10 +1330,10 @@
         <v>22</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1295,10 +1362,10 @@
         <v>22</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1327,10 +1394,10 @@
         <v>22</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1359,10 +1426,10 @@
         <v>22</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1391,10 +1458,10 @@
         <v>22</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1423,10 +1490,10 @@
         <v>22</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1455,10 +1522,10 @@
         <v>22</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1487,10 +1554,10 @@
         <v>22</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1519,10 +1586,10 @@
         <v>22</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1551,10 +1618,10 @@
         <v>22</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -1583,10 +1650,10 @@
         <v>22</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -1615,10 +1682,10 @@
         <v>22</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -1647,10 +1714,10 @@
         <v>22</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -1679,10 +1746,10 @@
         <v>22</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -1711,10 +1778,10 @@
         <v>22</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -1743,10 +1810,10 @@
         <v>22</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -1775,10 +1842,10 @@
         <v>22</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -1807,10 +1874,10 @@
         <v>22</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -1839,10 +1906,10 @@
         <v>22</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -1871,10 +1938,10 @@
         <v>22</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -1903,10 +1970,10 @@
         <v>22</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -1935,10 +2002,10 @@
         <v>22</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -1967,10 +2034,10 @@
         <v>22</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -1999,10 +2066,10 @@
         <v>22</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -2031,10 +2098,10 @@
         <v>22</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -2063,10 +2130,10 @@
         <v>22</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -2095,10 +2162,10 @@
         <v>22</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
@@ -2127,10 +2194,10 @@
         <v>22</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -2159,10 +2226,10 @@
         <v>22</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -2191,10 +2258,10 @@
         <v>22</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -2223,10 +2290,10 @@
         <v>22</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -2255,10 +2322,10 @@
         <v>22</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -2287,10 +2354,10 @@
         <v>22</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -2319,10 +2386,10 @@
         <v>22</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -2351,10 +2418,10 @@
         <v>22</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -2383,10 +2450,10 @@
         <v>22</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -2415,10 +2482,10 @@
         <v>22</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -2447,10 +2514,10 @@
         <v>22</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -2479,10 +2546,10 @@
         <v>22</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -2511,10 +2578,10 @@
         <v>22</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -2543,10 +2610,10 @@
         <v>22</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -2575,10 +2642,10 @@
         <v>22</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -2607,10 +2674,10 @@
         <v>22</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -2639,10 +2706,10 @@
         <v>22</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -2671,10 +2738,10 @@
         <v>22</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -2703,10 +2770,10 @@
         <v>22</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -2735,10 +2802,10 @@
         <v>22</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -2767,10 +2834,10 @@
         <v>22</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -2799,10 +2866,10 @@
         <v>22</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -2831,10 +2898,10 @@
         <v>22</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -2863,10 +2930,10 @@
         <v>22</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -2895,10 +2962,10 @@
         <v>22</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -2927,10 +2994,10 @@
         <v>22</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -2959,10 +3026,10 @@
         <v>22</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -2991,10 +3058,10 @@
         <v>22</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
@@ -3023,10 +3090,10 @@
         <v>22</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
@@ -3055,10 +3122,10 @@
         <v>22</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -3087,10 +3154,10 @@
         <v>22</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
@@ -3119,10 +3186,10 @@
         <v>22</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
@@ -3151,10 +3218,10 @@
         <v>22</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
@@ -3183,10 +3250,10 @@
         <v>22</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
@@ -3215,10 +3282,10 @@
         <v>22</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
@@ -3247,10 +3314,10 @@
         <v>22</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
@@ -3279,10 +3346,10 @@
         <v>22</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -3311,10 +3378,10 @@
         <v>22</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
@@ -3343,10 +3410,10 @@
         <v>22</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -3375,10 +3442,10 @@
         <v>22</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -3407,10 +3474,10 @@
         <v>22</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
@@ -3439,10 +3506,10 @@
         <v>22</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
@@ -3471,10 +3538,10 @@
         <v>22</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
@@ -3503,10 +3570,10 @@
         <v>22</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -3535,10 +3602,10 @@
         <v>22</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
@@ -3567,10 +3634,10 @@
         <v>22</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
@@ -3599,10 +3666,10 @@
         <v>22</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
@@ -3631,10 +3698,10 @@
         <v>22</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
@@ -3663,10 +3730,10 @@
         <v>22</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
@@ -3695,10 +3762,10 @@
         <v>22</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
@@ -3727,10 +3794,10 @@
         <v>22</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
@@ -3759,10 +3826,10 @@
         <v>22</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
@@ -3791,10 +3858,10 @@
         <v>22</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
@@ -3823,10 +3890,10 @@
         <v>22</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
@@ -3855,10 +3922,10 @@
         <v>22</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
@@ -3887,10 +3954,10 @@
         <v>22</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
@@ -3919,10 +3986,10 @@
         <v>22</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
@@ -3951,10 +4018,10 @@
         <v>22</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
@@ -3983,10 +4050,10 @@
         <v>22</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
@@ -4015,10 +4082,10 @@
         <v>22</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
@@ -4047,10 +4114,10 @@
         <v>22</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
@@ -4079,10 +4146,10 @@
         <v>22</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
@@ -4111,10 +4178,10 @@
         <v>22</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
@@ -4143,10 +4210,10 @@
         <v>22</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
@@ -4175,10 +4242,10 @@
         <v>22</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
@@ -4207,10 +4274,10 @@
         <v>22</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
@@ -4239,10 +4306,10 @@
         <v>22</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
@@ -6543,10 +6610,10 @@
         <v>0</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J187" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="188" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -6575,10 +6642,10 @@
         <v>0</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="189" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -6607,10 +6674,10 @@
         <v>0</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J189" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="190" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -6639,10 +6706,10 @@
         <v>0</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J190" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="191" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -6671,10 +6738,10 @@
         <v>0</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J191" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="192" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -6703,10 +6770,10 @@
         <v>0</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J192" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.3">
@@ -6735,10 +6802,10 @@
         <v>0</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J193" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>